<commit_message>
Edited user story description xsls
</commit_message>
<xml_diff>
--- a/DOCS/User Story Descriptions.xlsx
+++ b/DOCS/User Story Descriptions.xlsx
@@ -57,9 +57,6 @@
     <t>Question Mngnmnt</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Deleting</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Automated Question Paper Generator(AQPG) with Blooms Taxonomy Evaluation (V2)</t>
+  </si>
+  <si>
+    <t>DESCRIPTIONS</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,7 +652,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -664,7 +664,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -675,17 +675,17 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -693,12 +693,12 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -706,17 +706,17 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -724,12 +724,12 @@
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
@@ -740,12 +740,12 @@
         <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
@@ -753,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
@@ -761,12 +761,12 @@
         <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
@@ -777,12 +777,12 @@
         <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
@@ -790,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
@@ -798,12 +798,12 @@
         <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
@@ -814,12 +814,12 @@
         <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
@@ -827,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
@@ -835,12 +835,12 @@
         <v>9</v>
       </c>
       <c r="F44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
@@ -851,12 +851,12 @@
         <v>8</v>
       </c>
       <c r="F47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
@@ -864,7 +864,7 @@
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
@@ -872,69 +872,69 @@
         <v>9</v>
       </c>
       <c r="F52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
         <v>16</v>
       </c>
-      <c r="D61" t="s">
-        <v>17</v>
-      </c>
       <c r="F61" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>